<commit_message>
feat: MA department added to database
</commit_message>
<xml_diff>
--- a/data/courses_data.xlsx
+++ b/data/courses_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\course-finder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2218" documentId="13_ncr:1_{F59BF6A5-6A6E-45C1-A2CF-C3496E242A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8125880-6D50-407D-8FF2-CE3927C0C176}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C082D5-25BD-4C39-878D-B7FB271F468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="6570" windowWidth="18915" windowHeight="11400" activeTab="1" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
+    <workbookView xWindow="7185" yWindow="3630" windowWidth="18915" windowHeight="15525" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="FM - Finance" sheetId="3" r:id="rId1"/>
-    <sheet name="MG - Management" sheetId="4" r:id="rId2"/>
-    <sheet name="EC - Economics" sheetId="2" r:id="rId3"/>
-    <sheet name="GV - Government" sheetId="1" r:id="rId4"/>
+    <sheet name="MA - Mathematics" sheetId="6" r:id="rId1"/>
+    <sheet name="FM - Finance" sheetId="3" r:id="rId2"/>
+    <sheet name="MG - Management" sheetId="4" r:id="rId3"/>
+    <sheet name="EC - Economics" sheetId="2" r:id="rId4"/>
+    <sheet name="GV - Government" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="301">
   <si>
     <t>Code</t>
   </si>
@@ -774,16 +775,186 @@
   </si>
   <si>
     <t>The Politics and Policy of Climate Change and Sustainability</t>
+  </si>
+  <si>
+    <t>MA100</t>
+  </si>
+  <si>
+    <t>MA102</t>
+  </si>
+  <si>
+    <t>MA103</t>
+  </si>
+  <si>
+    <t>MA107</t>
+  </si>
+  <si>
+    <t>MA108</t>
+  </si>
+  <si>
+    <t>MA203</t>
+  </si>
+  <si>
+    <t>MA207</t>
+  </si>
+  <si>
+    <t>MA208</t>
+  </si>
+  <si>
+    <t>MA209</t>
+  </si>
+  <si>
+    <t>MA210</t>
+  </si>
+  <si>
+    <t>MA211</t>
+  </si>
+  <si>
+    <t>MA212</t>
+  </si>
+  <si>
+    <t>MA213</t>
+  </si>
+  <si>
+    <t>MA214</t>
+  </si>
+  <si>
+    <t>MA222</t>
+  </si>
+  <si>
+    <t>MA301</t>
+  </si>
+  <si>
+    <t>MA316</t>
+  </si>
+  <si>
+    <t>MA317</t>
+  </si>
+  <si>
+    <t>MA318</t>
+  </si>
+  <si>
+    <t>MA319</t>
+  </si>
+  <si>
+    <t>MA320</t>
+  </si>
+  <si>
+    <t>MA321</t>
+  </si>
+  <si>
+    <t>MA322</t>
+  </si>
+  <si>
+    <t>MA323</t>
+  </si>
+  <si>
+    <t>MA324</t>
+  </si>
+  <si>
+    <t>MA330</t>
+  </si>
+  <si>
+    <t>MA333</t>
+  </si>
+  <si>
+    <t>MA334</t>
+  </si>
+  <si>
+    <t>Mathematical Methods</t>
+  </si>
+  <si>
+    <t>Mathematical Proof and Analysis</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Mathematics</t>
+  </si>
+  <si>
+    <t>Quantitative Methods (Mathematics)</t>
+  </si>
+  <si>
+    <t>Methods in Calculus and Linear Algebra</t>
+  </si>
+  <si>
+    <t>Real Analysis</t>
+  </si>
+  <si>
+    <t>Further Quantitative Methods (Mathematics)</t>
+  </si>
+  <si>
+    <t>Optimisation Theory</t>
+  </si>
+  <si>
+    <t>Differential Equations</t>
+  </si>
+  <si>
+    <t>Discrete Mathematics</t>
+  </si>
+  <si>
+    <t>Algebra and Number Theory</t>
+  </si>
+  <si>
+    <t>Further Mathematical Methods</t>
+  </si>
+  <si>
+    <t>Operations Research Techniques</t>
+  </si>
+  <si>
+    <t>Algorithms and Data Structures</t>
+  </si>
+  <si>
+    <t>Further Mathematical Methods (Linear Algebra)</t>
+  </si>
+  <si>
+    <t>Mathematical Game Theory</t>
+  </si>
+  <si>
+    <t>Graph Theory</t>
+  </si>
+  <si>
+    <t>Complex Analysis</t>
+  </si>
+  <si>
+    <t>History and Culture of Mathematics</t>
+  </si>
+  <si>
+    <t>Partial Differential Equations</t>
+  </si>
+  <si>
+    <t>Mathematics of Networks</t>
+  </si>
+  <si>
+    <t>Measure Theoretic Probability</t>
+  </si>
+  <si>
+    <t>Mathematics of Finance and Valuation</t>
+  </si>
+  <si>
+    <t>Computational Methods in Financial Mathematics</t>
+  </si>
+  <si>
+    <t>Mathematical Modelling and Simulation</t>
+  </si>
+  <si>
+    <t>Game Theory for Collective Decisions</t>
+  </si>
+  <si>
+    <t>Optimisation for Machine Learning</t>
+  </si>
+  <si>
+    <t>Dissertation in Mathematics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +966,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -832,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,7 +1050,18 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1209,39 +1397,1706 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4289AE-5C21-47E6-BE9F-F3EB4C22DEB6}">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19">
+        <v>386</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="I2" s="17">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="J2" s="17">
+        <v>0.107</v>
+      </c>
+      <c r="K2" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>59.7</v>
+      </c>
+      <c r="M2" s="2">
+        <v>99</v>
+      </c>
+      <c r="N2" s="16">
+        <v>0</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="19">
+        <v>64</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.188</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="G3" s="17">
+        <v>0.188</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="I3" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="J3" s="17">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="K3" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>53</v>
+      </c>
+      <c r="M3" s="2">
+        <v>90</v>
+      </c>
+      <c r="N3" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0</v>
+      </c>
+      <c r="P3" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="19">
+        <v>167</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.218</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H4" s="17">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I4" s="17">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0.182</v>
+      </c>
+      <c r="K4" s="17">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>53.4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>93</v>
+      </c>
+      <c r="N4" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="19">
+        <v>465</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.372</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H5" s="17">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I5" s="17">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J5" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="K5" s="17">
+        <v>2.7E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>61.8</v>
+      </c>
+      <c r="M5" s="2">
+        <v>97</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0</v>
+      </c>
+      <c r="P5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="19">
+        <v>205</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.184</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0.107</v>
+      </c>
+      <c r="H6" s="17">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L6" s="2">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="M6" s="2">
+        <v>97</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="19">
+        <v>134</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="I7" s="17">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="K7" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>51.3</v>
+      </c>
+      <c r="M7" s="2">
+        <v>94</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="19">
+        <v>85</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.153</v>
+      </c>
+      <c r="H8" s="17">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J8" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K8" s="17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>63.9</v>
+      </c>
+      <c r="M8" s="2">
+        <v>91</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
+      <c r="P8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="19">
+        <v>59</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.186</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="I9" s="17">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J9" s="17">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="M9" s="2">
+        <v>96</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="19">
+        <v>94</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.253</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H10" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I10" s="17">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J10" s="17">
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L10" s="2">
+        <v>69.2</v>
+      </c>
+      <c r="M10" s="2">
+        <v>93</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="19">
+        <v>9</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.111</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>46.6</v>
+      </c>
+      <c r="M11" s="2">
+        <v>79</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="19">
+        <v>9</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0.111</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>61.6</v>
+      </c>
+      <c r="M12" s="2">
+        <v>83</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="19">
+        <v>255</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="I13" s="17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>56.1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>97</v>
+      </c>
+      <c r="N13" s="16">
+        <v>0</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0</v>
+      </c>
+      <c r="P13" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="19">
+        <v>212</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0.216</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="I14" s="17">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0.08</v>
+      </c>
+      <c r="K14" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L14" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>94</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0</v>
+      </c>
+      <c r="P14" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="19">
+        <v>47</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.128</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0.255</v>
+      </c>
+      <c r="H15" s="17">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>64.7</v>
+      </c>
+      <c r="M15" s="2">
+        <v>90</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B16" t="s">
+        <v>287</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="19">
+        <v>22</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.13</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="G16" s="17">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0.217</v>
+      </c>
+      <c r="I16" s="17">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0.217</v>
+      </c>
+      <c r="K16" s="17">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>48.8</v>
+      </c>
+      <c r="M16" s="2">
+        <v>71</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" t="s">
+        <v>288</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="19">
+        <v>76</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="G17" s="17">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="H17" s="17">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="M17" s="2">
+        <v>95</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="19">
+        <v>8</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.375</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="H18" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>59.4</v>
+      </c>
+      <c r="M18" s="2">
+        <v>83</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="19">
+        <v>14</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="F19" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="H19" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="I19" s="17">
+        <v>0</v>
+      </c>
+      <c r="J19" s="17">
+        <v>0</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>61.8</v>
+      </c>
+      <c r="M19" s="2">
+        <v>85</v>
+      </c>
+      <c r="N19" s="16">
+        <v>0</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0</v>
+      </c>
+      <c r="P19" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="B20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="19">
+        <v>12</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G20" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H20" s="17">
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>65.3</v>
+      </c>
+      <c r="M20" s="2">
+        <v>75</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="19">
+        <v>12</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="G21" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="M21" s="2">
+        <v>79</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0</v>
+      </c>
+      <c r="P21" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" t="s">
+        <v>293</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="19">
+        <v>5</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>71.8</v>
+      </c>
+      <c r="M22" s="2">
+        <v>78</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0</v>
+      </c>
+      <c r="O22" s="16">
+        <v>0</v>
+      </c>
+      <c r="P22" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B23" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="19">
+        <v>19</v>
+      </c>
+      <c r="E23" s="17">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="G23" s="17">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="H23" s="17">
+        <v>0.105</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>60.3</v>
+      </c>
+      <c r="M23" s="2">
+        <v>84</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0</v>
+      </c>
+      <c r="O23" s="16">
+        <v>0</v>
+      </c>
+      <c r="P23" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" t="s">
+        <v>295</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="19">
+        <v>15</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="F24" s="17">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G24" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H24" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="I24" s="17">
+        <v>0</v>
+      </c>
+      <c r="J24" s="17">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="K24" s="17">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>61.9</v>
+      </c>
+      <c r="M24" s="2">
+        <v>99</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0</v>
+      </c>
+      <c r="O24" s="16">
+        <v>0</v>
+      </c>
+      <c r="P24" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B25" t="s">
+        <v>296</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="19">
+        <v>28</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="F25" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G25" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="H25" s="17">
+        <v>0</v>
+      </c>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+      <c r="J25" s="17">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="K25" s="17">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="M25" s="2">
+        <v>93</v>
+      </c>
+      <c r="N25" s="16">
+        <v>1</v>
+      </c>
+      <c r="O25" s="16">
+        <v>0</v>
+      </c>
+      <c r="P25" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>1</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="19">
+        <v>40</v>
+      </c>
+      <c r="E26" s="17">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G26" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L26" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="M26" s="2">
+        <v>77</v>
+      </c>
+      <c r="N26" s="16">
+        <v>1</v>
+      </c>
+      <c r="O26" s="16">
+        <v>0</v>
+      </c>
+      <c r="P26" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>1</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="19">
+        <v>18</v>
+      </c>
+      <c r="E27" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="F27" s="17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G27" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="K27" s="17">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>46.2</v>
+      </c>
+      <c r="M27" s="2">
+        <v>87</v>
+      </c>
+      <c r="N27" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O27" s="16">
+        <v>0</v>
+      </c>
+      <c r="P27" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>1</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="19">
+        <v>7</v>
+      </c>
+      <c r="E28" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G28" s="17">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="H28" s="17">
+        <v>0</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
+      <c r="J28" s="17">
+        <v>0</v>
+      </c>
+      <c r="K28" s="17">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>62.4</v>
+      </c>
+      <c r="M28" s="2">
+        <v>75</v>
+      </c>
+      <c r="N28" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+      <c r="P28" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" t="s">
+        <v>300</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="19">
+        <v>10</v>
+      </c>
+      <c r="E29" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="G29" s="17">
+        <v>0</v>
+      </c>
+      <c r="H29" s="17">
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="17">
+        <v>0</v>
+      </c>
+      <c r="K29" s="17">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>71</v>
+      </c>
+      <c r="M29" s="2">
+        <v>91</v>
+      </c>
+      <c r="N29" s="16">
+        <v>1</v>
+      </c>
+      <c r="O29" s="16">
+        <v>0</v>
+      </c>
+      <c r="P29" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>2</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R29">
+    <sortCondition ref="A2:A29"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B1F18-5F75-47B1-B429-DF58E6F9E79C}">
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="T20" sqref="T20"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625"/>
     <col min="20" max="20" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +3152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
@@ -1310,25 +3165,25 @@
       <c r="D2" s="2">
         <v>65</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="17">
         <v>0.44600000000000001</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="17">
         <v>0.26200000000000001</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="18">
         <v>0.2</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="18">
         <v>6.2E-2</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="18">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="18">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="18">
         <v>0</v>
       </c>
       <c r="L2" s="1">
@@ -1353,7 +3208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
@@ -1366,25 +3221,25 @@
       <c r="D3" s="2">
         <v>471</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="17">
         <v>0.32100000000000001</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="17">
         <v>0.35</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="18">
         <v>0.16600000000000001</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="18">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="18">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="18">
         <v>5.5E-2</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="18">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="L3" s="1">
@@ -1409,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>22</v>
       </c>
@@ -1422,25 +3277,25 @@
       <c r="D4" s="2">
         <v>63</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="17">
         <v>0.41299999999999998</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="17">
         <v>0.38100000000000001</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="18">
         <v>0.127</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="18">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="I4" s="11">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0</v>
-      </c>
-      <c r="K4" s="11">
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="K4" s="18">
         <v>0</v>
       </c>
       <c r="L4" s="1">
@@ -1465,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>24</v>
       </c>
@@ -1478,25 +3333,25 @@
       <c r="D5" s="2">
         <v>69</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="17">
         <v>0.39100000000000001</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="17">
         <v>0.246</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="18">
         <v>0.23200000000000001</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="18">
         <v>0.13</v>
       </c>
-      <c r="I5" s="11">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0</v>
-      </c>
-      <c r="K5" s="11">
+      <c r="I5" s="18">
+        <v>0</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
         <v>0</v>
       </c>
       <c r="L5" s="1">
@@ -1521,7 +3376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
@@ -1534,25 +3389,25 @@
       <c r="D6" s="2">
         <v>68</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="17">
         <v>0.33800000000000002</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="17">
         <v>0.47099999999999997</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="18">
         <v>0.11799999999999999</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="18">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="I6" s="11">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11">
+      <c r="I6" s="18">
+        <v>0</v>
+      </c>
+      <c r="J6" s="18">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="18">
         <v>0</v>
       </c>
       <c r="L6" s="1">
@@ -1577,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>28</v>
       </c>
@@ -1590,25 +3445,25 @@
       <c r="D7" s="2">
         <v>186</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="17">
         <v>0.23699999999999999</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="17">
         <v>0.30599999999999999</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="18">
         <v>0.28499999999999998</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="18">
         <v>0.11799999999999999</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="18">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="18">
         <v>2.7E-2</v>
       </c>
       <c r="L7" s="1">
@@ -1633,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
@@ -1646,25 +3501,25 @@
       <c r="D8" s="2">
         <v>449</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="17">
         <v>0.19400000000000001</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="17">
         <v>0.25800000000000001</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="18">
         <v>0.25600000000000001</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="18">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="18">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="18">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="18">
         <v>1.6E-2</v>
       </c>
       <c r="L8" s="1">
@@ -1689,7 +3544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
@@ -1702,25 +3557,25 @@
       <c r="D9" s="2">
         <v>219</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="17">
         <v>0.41099999999999998</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="17">
         <v>0.30099999999999999</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="18">
         <v>0.21</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="18">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I9" s="11">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18">
         <v>2.7E-2</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="18">
         <v>0</v>
       </c>
       <c r="L9" s="1">
@@ -1745,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
@@ -1758,25 +3613,25 @@
       <c r="D10" s="2">
         <v>49</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="17">
         <v>0.40799999999999997</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="17">
         <v>0.55100000000000005</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="18">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="11">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11">
-        <v>0</v>
-      </c>
-      <c r="K10" s="11">
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18">
         <v>0</v>
       </c>
       <c r="L10" s="1">
@@ -1801,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>35</v>
       </c>
@@ -1814,25 +3669,25 @@
       <c r="D11" s="2">
         <v>48</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="17">
         <v>0.27100000000000002</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="17">
         <v>0.58299999999999996</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="18">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H11" s="11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
+      <c r="H11" s="18">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18">
         <v>0</v>
       </c>
       <c r="L11" s="1">
@@ -1857,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>37</v>
       </c>
@@ -1870,25 +3725,25 @@
       <c r="D12" s="2">
         <v>49</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="17">
         <v>0.32700000000000001</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="17">
         <v>0.38800000000000001</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="18">
         <v>0.245</v>
       </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
-        <v>0</v>
-      </c>
-      <c r="J12" s="11">
+      <c r="H12" s="18">
+        <v>0</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0</v>
+      </c>
+      <c r="J12" s="18">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="18">
         <v>0</v>
       </c>
       <c r="L12" s="1">
@@ -1913,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
@@ -1926,25 +3781,25 @@
       <c r="D13" s="2">
         <v>48</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="17">
         <v>0.33300000000000002</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="17">
         <v>0.375</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="18">
         <v>0.20799999999999999</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="18">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="I13" s="11">
-        <v>0</v>
-      </c>
-      <c r="J13" s="11">
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
         <v>6.2E-2</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="18">
         <v>0</v>
       </c>
       <c r="L13" s="1">
@@ -1969,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>41</v>
       </c>
@@ -1982,25 +3837,25 @@
       <c r="D14" s="2">
         <v>148</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="17">
         <v>0.34499999999999997</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="17">
         <v>0.5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="18">
         <v>0.128</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="18">
         <v>0.02</v>
       </c>
-      <c r="I14" s="11">
-        <v>0</v>
-      </c>
-      <c r="J14" s="11">
-        <v>0</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="L14" s="1">
@@ -2025,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
@@ -2038,25 +3893,25 @@
       <c r="D15" s="2">
         <v>124</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="17">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="17">
         <v>0.33900000000000002</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="18">
         <v>0.17699999999999999</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="18">
         <v>0.13700000000000001</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="18">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="18">
         <v>0.04</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="18">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="L15" s="1">
@@ -2081,122 +3936,122 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="14:16">
+    <row r="17" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="14:16">
+    <row r="18" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="14:16">
+    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="14:16">
+    <row r="20" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="14:16">
+    <row r="21" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="14:16">
+    <row r="22" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="14:16">
+    <row r="23" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="14:16">
+    <row r="24" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="14:16">
+    <row r="25" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="14:16">
+    <row r="26" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="14:16">
+    <row r="27" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="14:16">
+    <row r="28" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="14:16">
+    <row r="29" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="14:16">
+    <row r="30" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="14:16">
+    <row r="31" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="14:16">
+    <row r="32" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="14:16">
+    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="14:16">
+    <row r="34" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="14:16">
+    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="14:16">
+    <row r="36" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="14:16">
+    <row r="37" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="14:16">
+    <row r="38" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="14:16">
+    <row r="39" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -2206,18 +4061,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E33BB37-4D69-4A58-80FE-648AC47B185D}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="Q27" sqref="Q27"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
@@ -2239,7 +4094,7 @@
     <col min="20" max="20" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +4150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>45</v>
       </c>
@@ -2351,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
@@ -2407,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>49</v>
       </c>
@@ -2463,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>51</v>
       </c>
@@ -2519,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>53</v>
       </c>
@@ -2575,7 +4430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>55</v>
       </c>
@@ -2631,7 +4486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>57</v>
       </c>
@@ -2687,7 +4542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>59</v>
       </c>
@@ -2743,7 +4598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>61</v>
       </c>
@@ -2799,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>63</v>
       </c>
@@ -2855,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>65</v>
       </c>
@@ -2911,7 +4766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>67</v>
       </c>
@@ -2967,7 +4822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>69</v>
       </c>
@@ -3023,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -3079,7 +4934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>73</v>
       </c>
@@ -3135,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>75</v>
       </c>
@@ -3191,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>77</v>
       </c>
@@ -3247,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>79</v>
       </c>
@@ -3303,7 +5158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>81</v>
       </c>
@@ -3359,7 +5214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>83</v>
       </c>
@@ -3415,7 +5270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>85</v>
       </c>
@@ -3471,89 +5326,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="14"/>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="14"/>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="14"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="14"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="14"/>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="14"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="14"/>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="14"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="14"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="14"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="14"/>
+    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="14"/>
+    <row r="34" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
@@ -3563,18 +5406,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}">
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
@@ -3596,7 +5439,7 @@
     <col min="20" max="20" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3652,7 +5495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>87</v>
       </c>
@@ -3708,7 +5551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
@@ -3764,7 +5607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>90</v>
       </c>
@@ -3820,7 +5663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>91</v>
       </c>
@@ -3876,7 +5719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>93</v>
       </c>
@@ -3932,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>94</v>
       </c>
@@ -3988,7 +5831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>95</v>
       </c>
@@ -4044,7 +5887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>97</v>
       </c>
@@ -4100,7 +5943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>99</v>
       </c>
@@ -4156,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>101</v>
       </c>
@@ -4212,7 +6055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>103</v>
       </c>
@@ -4268,7 +6111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>104</v>
       </c>
@@ -4324,7 +6167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>105</v>
       </c>
@@ -4380,7 +6223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>107</v>
       </c>
@@ -4436,7 +6279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>108</v>
       </c>
@@ -4492,7 +6335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>109</v>
       </c>
@@ -4548,7 +6391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>111</v>
       </c>
@@ -4604,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>112</v>
       </c>
@@ -4660,7 +6503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>113</v>
       </c>
@@ -4716,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>115</v>
       </c>
@@ -4772,7 +6615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>117</v>
       </c>
@@ -4828,7 +6671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>119</v>
       </c>
@@ -4884,7 +6727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>121</v>
       </c>
@@ -4940,7 +6783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>123</v>
       </c>
@@ -4996,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>125</v>
       </c>
@@ -5052,7 +6895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>127</v>
       </c>
@@ -5108,7 +6951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>129</v>
       </c>
@@ -5164,7 +7007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>131</v>
       </c>
@@ -5220,7 +7063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>133</v>
       </c>
@@ -5276,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>135</v>
       </c>
@@ -5332,7 +7175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>137</v>
       </c>
@@ -5388,7 +7231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>139</v>
       </c>
@@ -5444,7 +7287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>141</v>
       </c>
@@ -5500,7 +7343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>143</v>
       </c>
@@ -5556,22 +7399,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -5584,18 +7427,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD98AB24-8EFF-4477-9EFD-02014029C60E}">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.42578125" bestFit="1" customWidth="1"/>
@@ -5615,7 +7458,7 @@
     <col min="20" max="20" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5671,7 +7514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -5727,7 +7570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>148</v>
       </c>
@@ -5783,7 +7626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>151</v>
       </c>
@@ -5839,7 +7682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>154</v>
       </c>
@@ -5895,7 +7738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>157</v>
       </c>
@@ -5951,7 +7794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>160</v>
       </c>
@@ -6007,7 +7850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>163</v>
       </c>
@@ -6063,7 +7906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>166</v>
       </c>
@@ -6119,7 +7962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>170</v>
       </c>
@@ -6175,7 +8018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>173</v>
       </c>
@@ -6231,7 +8074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>176</v>
       </c>
@@ -6287,7 +8130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>178</v>
       </c>
@@ -6343,7 +8186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>180</v>
       </c>
@@ -6399,7 +8242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>183</v>
       </c>
@@ -6455,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>186</v>
       </c>
@@ -6511,7 +8354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>189</v>
       </c>
@@ -6567,7 +8410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>192</v>
       </c>
@@ -6623,7 +8466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>195</v>
       </c>
@@ -6679,7 +8522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>197</v>
       </c>
@@ -6735,7 +8578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>199</v>
       </c>
@@ -6791,7 +8634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>201</v>
       </c>
@@ -6847,7 +8690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>203</v>
       </c>
@@ -6903,7 +8746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>205</v>
       </c>
@@ -6959,7 +8802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>207</v>
       </c>
@@ -7015,7 +8858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>209</v>
       </c>
@@ -7071,7 +8914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>211</v>
       </c>
@@ -7127,7 +8970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>213</v>
       </c>
@@ -7183,7 +9026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>215</v>
       </c>
@@ -7239,7 +9082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>217</v>
       </c>
@@ -7295,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>219</v>
       </c>
@@ -7351,7 +9194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>221</v>
       </c>
@@ -7407,7 +9250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>223</v>
       </c>
@@ -7463,7 +9306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>225</v>
       </c>
@@ -7519,7 +9362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>227</v>
       </c>
@@ -7575,7 +9418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>229</v>
       </c>
@@ -7631,7 +9474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>231</v>
       </c>
@@ -7687,7 +9530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>233</v>
       </c>
@@ -7743,7 +9586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>235</v>
       </c>
@@ -7799,7 +9642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>237</v>
       </c>
@@ -7855,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>239</v>
       </c>
@@ -7911,7 +9754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>241</v>
       </c>
@@ -7967,7 +9810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>243</v>
       </c>

</xml_diff>

<commit_message>
feat: IR department added to database
</commit_message>
<xml_diff>
--- a/data/courses_data.xlsx
+++ b/data/courses_data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\course-finder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C082D5-25BD-4C39-878D-B7FB271F468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7154E834-E182-4F9A-8B97-F340CA1CF3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="3630" windowWidth="18915" windowHeight="15525" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
+    <workbookView xWindow="1590" yWindow="2925" windowWidth="17640" windowHeight="15525" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="MA - Mathematics" sheetId="6" r:id="rId1"/>
-    <sheet name="FM - Finance" sheetId="3" r:id="rId2"/>
-    <sheet name="MG - Management" sheetId="4" r:id="rId3"/>
-    <sheet name="EC - Economics" sheetId="2" r:id="rId4"/>
-    <sheet name="GV - Government" sheetId="1" r:id="rId5"/>
+    <sheet name="IR - International Relations" sheetId="7" r:id="rId1"/>
+    <sheet name="MA - Mathematics" sheetId="6" r:id="rId2"/>
+    <sheet name="FM - Finance" sheetId="3" r:id="rId3"/>
+    <sheet name="MG - Management" sheetId="4" r:id="rId4"/>
+    <sheet name="EC - Economics" sheetId="2" r:id="rId5"/>
+    <sheet name="GV - Government" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="355">
   <si>
     <t>Code</t>
   </si>
@@ -943,6 +944,168 @@
   </si>
   <si>
     <t>Dissertation in Mathematics</t>
+  </si>
+  <si>
+    <t>IR100</t>
+  </si>
+  <si>
+    <t>IR101</t>
+  </si>
+  <si>
+    <t>IR200</t>
+  </si>
+  <si>
+    <t>IR202</t>
+  </si>
+  <si>
+    <t>IR203</t>
+  </si>
+  <si>
+    <t>IR205</t>
+  </si>
+  <si>
+    <t>IR206</t>
+  </si>
+  <si>
+    <t>IR305</t>
+  </si>
+  <si>
+    <t>IR312</t>
+  </si>
+  <si>
+    <t>IR314</t>
+  </si>
+  <si>
+    <t>IR315</t>
+  </si>
+  <si>
+    <t>International Relations of the Middle East</t>
+  </si>
+  <si>
+    <t>International Relations: Theories, Concepts and Debates</t>
+  </si>
+  <si>
+    <t>Contemporary Issues in International Relations</t>
+  </si>
+  <si>
+    <t>International Political Theory</t>
+  </si>
+  <si>
+    <t>Foreign Policy Analysis I</t>
+  </si>
+  <si>
+    <t>International Security</t>
+  </si>
+  <si>
+    <t>International Political Economy</t>
+  </si>
+  <si>
+    <t>Strategic Aspects of International Relations</t>
+  </si>
+  <si>
+    <t>Genocide</t>
+  </si>
+  <si>
+    <t>International Organisations</t>
+  </si>
+  <si>
+    <t>Southeast Asia: Intra-regional Politics and Security</t>
+  </si>
+  <si>
+    <t>IR317</t>
+  </si>
+  <si>
+    <t>American Grand Strategy</t>
+  </si>
+  <si>
+    <t>IR318</t>
+  </si>
+  <si>
+    <t>Visual International Politics</t>
+  </si>
+  <si>
+    <t>IR323</t>
+  </si>
+  <si>
+    <t>Race and Gender in International Relations</t>
+  </si>
+  <si>
+    <t>IR327</t>
+  </si>
+  <si>
+    <t>World Orders in Historical International Relations</t>
+  </si>
+  <si>
+    <t>Conflict and Peacebuilding</t>
+  </si>
+  <si>
+    <t>IR354</t>
+  </si>
+  <si>
+    <t>Governing International Political Economy: Lessons from the Past for the Future</t>
+  </si>
+  <si>
+    <t>IR367</t>
+  </si>
+  <si>
+    <t>Political Economy of Climate Change</t>
+  </si>
+  <si>
+    <t>IR368</t>
+  </si>
+  <si>
+    <t>The Political Economy of Trade</t>
+  </si>
+  <si>
+    <t>IR369</t>
+  </si>
+  <si>
+    <t>Politics of Money in the World Economy</t>
+  </si>
+  <si>
+    <t>IR373</t>
+  </si>
+  <si>
+    <t>China and the Global South</t>
+  </si>
+  <si>
+    <t>IR374</t>
+  </si>
+  <si>
+    <t>IR377</t>
+  </si>
+  <si>
+    <t>The Politics of Peace and Security in Sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>IR379</t>
+  </si>
+  <si>
+    <t>Eastern Europe: Domestic Regimes and Foregin Policies</t>
+  </si>
+  <si>
+    <t>IR380</t>
+  </si>
+  <si>
+    <t>The Politics of Inequality and Development</t>
+  </si>
+  <si>
+    <t>IR391</t>
+  </si>
+  <si>
+    <t>Globalisation and Development</t>
+  </si>
+  <si>
+    <t>IR395</t>
+  </si>
+  <si>
+    <t>The Politics of Displacement and Refuge</t>
+  </si>
+  <si>
+    <t>IR398</t>
+  </si>
+  <si>
+    <t>Dissertation</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1064,6 +1227,26 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1397,10 +1580,1674 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1DA8C1-C587-45DF-87D3-9DC3B52B43A1}">
+  <dimension ref="A1:R32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="12" style="17" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="67.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>118</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.127</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="H2" s="17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J2" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K2" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L2" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="M2" s="2">
+        <v>77</v>
+      </c>
+      <c r="N2" s="16">
+        <v>1</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>68</v>
+      </c>
+      <c r="E3" s="17">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="G3" s="17">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>0</v>
+      </c>
+      <c r="J3" s="17">
+        <v>0</v>
+      </c>
+      <c r="K3" s="17">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>64.3</v>
+      </c>
+      <c r="M3" s="2">
+        <v>72</v>
+      </c>
+      <c r="N3" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>25</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.32</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.12</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0</v>
+      </c>
+      <c r="K4" s="17">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>66.2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>78</v>
+      </c>
+      <c r="N4" s="16">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>136</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H5" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0</v>
+      </c>
+      <c r="J5" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K5" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>63.3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>77</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0</v>
+      </c>
+      <c r="P5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>62</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G6" s="17">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>70.5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>83</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>123</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0.106</v>
+      </c>
+      <c r="H7" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>66.2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>78</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>122</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H8" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I8" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J8" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K8" s="17">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>64.3</v>
+      </c>
+      <c r="M8" s="2">
+        <v>84</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0.65</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
+      <c r="P8" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>36</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="G9" s="17">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="H9" s="17">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>67.5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>77</v>
+      </c>
+      <c r="N9" s="16">
+        <v>1</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>28</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="G10" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>67.3</v>
+      </c>
+      <c r="M10" s="2">
+        <v>77</v>
+      </c>
+      <c r="N10" s="16">
+        <v>1</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>13</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.308</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H11" s="17">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>77</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>35</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.314</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0.114</v>
+      </c>
+      <c r="H12" s="17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>65.8</v>
+      </c>
+      <c r="M12" s="2">
+        <v>74</v>
+      </c>
+      <c r="N12" s="16">
+        <v>1</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>30</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="H13" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0</v>
+      </c>
+      <c r="K13" s="17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>60.8</v>
+      </c>
+      <c r="M13" s="2">
+        <v>74</v>
+      </c>
+      <c r="N13" s="16">
+        <v>1</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0</v>
+      </c>
+      <c r="P13" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>14</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="M14" s="2">
+        <v>83</v>
+      </c>
+      <c r="N14" s="16">
+        <v>1</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0</v>
+      </c>
+      <c r="P14" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>2</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>19</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>68.8</v>
+      </c>
+      <c r="M15" s="2">
+        <v>77</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>15</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="G16" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>66.8</v>
+      </c>
+      <c r="M16" s="2">
+        <v>78</v>
+      </c>
+      <c r="N16" s="16">
+        <v>1</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>7</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G17" s="17">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M17" s="2">
+        <v>73</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>26</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.308</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0.154</v>
+      </c>
+      <c r="H18" s="17">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>66.3</v>
+      </c>
+      <c r="M18" s="2">
+        <v>80</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>17</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="H19" s="17">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="I19" s="17">
+        <v>0</v>
+      </c>
+      <c r="J19" s="17">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>61.8</v>
+      </c>
+      <c r="M19" s="2">
+        <v>72</v>
+      </c>
+      <c r="N19" s="16">
+        <v>1</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0</v>
+      </c>
+      <c r="P19" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>24</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="H20" s="17">
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>65.8</v>
+      </c>
+      <c r="M20" s="2">
+        <v>72</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>14</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="G21" s="17">
+        <v>0.214</v>
+      </c>
+      <c r="H21" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>66</v>
+      </c>
+      <c r="M21" s="2">
+        <v>81</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0</v>
+      </c>
+      <c r="P21" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>42</v>
+      </c>
+      <c r="E22" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="H22" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>60.6</v>
+      </c>
+      <c r="M22" s="2">
+        <v>75</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="O22" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="P22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>13</v>
+      </c>
+      <c r="E23" s="17">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="G23" s="17">
+        <v>0</v>
+      </c>
+      <c r="H23" s="17">
+        <v>0</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="M23" s="2">
+        <v>75</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0</v>
+      </c>
+      <c r="O23" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="P23" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>16</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0.312</v>
+      </c>
+      <c r="F24" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="H24" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I24" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="J24" s="17">
+        <v>0</v>
+      </c>
+      <c r="K24" s="17">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>64.8</v>
+      </c>
+      <c r="M24" s="2">
+        <v>78</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="O24" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="P24" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>1</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>16</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="17">
+        <v>0</v>
+      </c>
+      <c r="H25" s="17">
+        <v>0</v>
+      </c>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+      <c r="J25" s="17">
+        <v>0</v>
+      </c>
+      <c r="K25" s="17">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>69.2</v>
+      </c>
+      <c r="M25" s="2">
+        <v>75</v>
+      </c>
+      <c r="N25" s="16">
+        <v>1</v>
+      </c>
+      <c r="O25" s="16">
+        <v>0</v>
+      </c>
+      <c r="P25" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>2</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>13</v>
+      </c>
+      <c r="E26" s="17">
+        <v>0.308</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G26" s="17">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>68.5</v>
+      </c>
+      <c r="M26" s="2">
+        <v>80</v>
+      </c>
+      <c r="N26" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O26" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P26" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>1</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>15</v>
+      </c>
+      <c r="E27" s="17">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="F27" s="17">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G27" s="17">
+        <v>0</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="K27" s="17">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="M27" s="2">
+        <v>74</v>
+      </c>
+      <c r="N27" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="O27" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="P27" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>1</v>
+      </c>
+      <c r="R27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>36</v>
+      </c>
+      <c r="E28" s="17">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="G28" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H28" s="17">
+        <v>0</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
+      <c r="J28" s="17">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="K28" s="17">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="L28" s="2">
+        <v>66.3</v>
+      </c>
+      <c r="M28" s="2">
+        <v>80</v>
+      </c>
+      <c r="N28" s="16">
+        <v>1</v>
+      </c>
+      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+      <c r="P28" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="22"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+    </row>
+    <row r="30" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="22"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+    </row>
+    <row r="31" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="22"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4289AE-5C21-47E6-BE9F-F3EB4C22DEB6}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -3061,7 +4908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B1F18-5F75-47B1-B429-DF58E6F9E79C}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -4061,7 +5908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E33BB37-4D69-4A58-80FE-648AC47B185D}">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -5406,7 +7253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -7427,12 +9274,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD98AB24-8EFF-4477-9EFD-02014029C60E}">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>

</xml_diff>

<commit_message>
add ST department to database
</commit_message>
<xml_diff>
--- a/data/courses_data.xlsx
+++ b/data/courses_data.xlsx
@@ -8,18 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\course-finder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7154E834-E182-4F9A-8B97-F340CA1CF3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD7728E-06E4-4E0A-A4CF-E8C1EAD49AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="2925" windowWidth="17640" windowHeight="15525" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
+    <workbookView xWindow="1590" yWindow="2925" windowWidth="17610" windowHeight="15525" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="IR - International Relations" sheetId="7" r:id="rId1"/>
-    <sheet name="MA - Mathematics" sheetId="6" r:id="rId2"/>
-    <sheet name="FM - Finance" sheetId="3" r:id="rId3"/>
-    <sheet name="MG - Management" sheetId="4" r:id="rId4"/>
-    <sheet name="EC - Economics" sheetId="2" r:id="rId5"/>
-    <sheet name="GV - Government" sheetId="1" r:id="rId6"/>
+    <sheet name="ST - Statistics" sheetId="9" r:id="rId1"/>
+    <sheet name="IR - International Relations" sheetId="7" r:id="rId2"/>
+    <sheet name="MA - Mathematics" sheetId="6" r:id="rId3"/>
+    <sheet name="FM - Finance" sheetId="3" r:id="rId4"/>
+    <sheet name="MG - Management" sheetId="4" r:id="rId5"/>
+    <sheet name="EC - Economics" sheetId="2" r:id="rId6"/>
+    <sheet name="GV - Government" sheetId="1" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'EC - Economics'!$A$1:$R$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FM - Finance'!$A$1:$R$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'GV - Government'!$A$1:$R$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'IR - International Relations'!$A$1:$R$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MA - Mathematics'!$A$1:$R$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'MG - Management'!$A$1:$R$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ST - Statistics'!$A$1:$R$31</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="417">
   <si>
     <t>Code</t>
   </si>
@@ -1106,6 +1116,192 @@
   </si>
   <si>
     <t>Dissertation</t>
+  </si>
+  <si>
+    <t>ST101</t>
+  </si>
+  <si>
+    <t>Programming for Data Science</t>
+  </si>
+  <si>
+    <t>ST102</t>
+  </si>
+  <si>
+    <t>Elementary Statistical Theory</t>
+  </si>
+  <si>
+    <t>ST107</t>
+  </si>
+  <si>
+    <t>Quantitative Methods (Statistics)</t>
+  </si>
+  <si>
+    <t>ST109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementary Statistical Theory I </t>
+  </si>
+  <si>
+    <t>ST115</t>
+  </si>
+  <si>
+    <t>Managing and Visualising Data</t>
+  </si>
+  <si>
+    <t>ST201</t>
+  </si>
+  <si>
+    <t>Statistical Models and Data Analysis</t>
+  </si>
+  <si>
+    <t>ST202</t>
+  </si>
+  <si>
+    <t>Probability, Distribution Theory and Inference</t>
+  </si>
+  <si>
+    <t>ST205</t>
+  </si>
+  <si>
+    <t>Sample Surveys and Experiments</t>
+  </si>
+  <si>
+    <t>ST206</t>
+  </si>
+  <si>
+    <t>Probability and Distribution Theory</t>
+  </si>
+  <si>
+    <t>ST207</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>ST211</t>
+  </si>
+  <si>
+    <t>Applied Regression</t>
+  </si>
+  <si>
+    <t>ST213</t>
+  </si>
+  <si>
+    <t>Introduction to Pricing, Hedging and Optimisation</t>
+  </si>
+  <si>
+    <t>Actuarial Investigations: Financial</t>
+  </si>
+  <si>
+    <t>ST227</t>
+  </si>
+  <si>
+    <t>Survival Models</t>
+  </si>
+  <si>
+    <t>ST300</t>
+  </si>
+  <si>
+    <t>Regression and Generalised Linear Models</t>
+  </si>
+  <si>
+    <t>ST301</t>
+  </si>
+  <si>
+    <t>ST302</t>
+  </si>
+  <si>
+    <t>Stochastic Processes</t>
+  </si>
+  <si>
+    <t>ST303</t>
+  </si>
+  <si>
+    <t>Stochastic Simulation</t>
+  </si>
+  <si>
+    <t>ST304</t>
+  </si>
+  <si>
+    <t>Time Series and Forecasting</t>
+  </si>
+  <si>
+    <t>ST306</t>
+  </si>
+  <si>
+    <t>Actuarial Mathematics (General)</t>
+  </si>
+  <si>
+    <t>Actuarial Mathematics (Life)</t>
+  </si>
+  <si>
+    <t>ST307</t>
+  </si>
+  <si>
+    <t>Aspects of Market Research</t>
+  </si>
+  <si>
+    <t>ST308</t>
+  </si>
+  <si>
+    <t>Bayesian Inference</t>
+  </si>
+  <si>
+    <t>ST309</t>
+  </si>
+  <si>
+    <t>Elementary Data Analytics</t>
+  </si>
+  <si>
+    <t>ST310</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>ST311</t>
+  </si>
+  <si>
+    <t>Artifical Intelligence</t>
+  </si>
+  <si>
+    <t>ST312</t>
+  </si>
+  <si>
+    <t>Applied Statistics Projects</t>
+  </si>
+  <si>
+    <t>ST313</t>
+  </si>
+  <si>
+    <t>Ethics for Data Science</t>
+  </si>
+  <si>
+    <t>ST314</t>
+  </si>
+  <si>
+    <t>Multilevel and Longitudinal Models</t>
+  </si>
+  <si>
+    <t>ST326</t>
+  </si>
+  <si>
+    <t>Financial Statistics</t>
+  </si>
+  <si>
+    <t>ST327</t>
+  </si>
+  <si>
+    <t>Market Research: An Integrated Approach</t>
+  </si>
+  <si>
+    <t>ST330</t>
+  </si>
+  <si>
+    <t>Stochastic and Actuarial Methods in Finance</t>
+  </si>
+  <si>
+    <t>ST226</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1239,14 +1435,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1580,31 +1782,1868 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1DA8C1-C587-45DF-87D3-9DC3B52B43A1}">
-  <dimension ref="A1:R32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}">
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
+      <selection pane="bottomRight" activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="12" style="17" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>89</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="H2" s="18">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I2" s="18">
+        <v>0</v>
+      </c>
+      <c r="J2" s="18">
+        <v>0.112</v>
+      </c>
+      <c r="K2" s="18">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>59.3</v>
+      </c>
+      <c r="M2" s="1">
+        <v>94</v>
+      </c>
+      <c r="N2" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19">
+        <v>386</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="G3" s="17">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0.161</v>
+      </c>
+      <c r="I3" s="17">
+        <v>3.9E-2</v>
+      </c>
+      <c r="J3" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="K3" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L3" s="2">
+        <v>59.7</v>
+      </c>
+      <c r="M3" s="2">
+        <v>100</v>
+      </c>
+      <c r="N3" s="16">
+        <v>0</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0</v>
+      </c>
+      <c r="P3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="B4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="19">
+        <v>466</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.161</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="H4" s="17">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="I4" s="17">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J4" s="17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K4" s="17">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>69.8</v>
+      </c>
+      <c r="M4" s="2">
+        <v>100</v>
+      </c>
+      <c r="N4" s="16">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" t="s">
+        <v>362</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="19">
+        <v>182</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.126</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.126</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="I5" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J5" s="17">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="K5" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>62.3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>100</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0</v>
+      </c>
+      <c r="P5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="B6" t="s">
+        <v>364</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="19">
+        <v>69</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G6" s="17">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>1.4E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>69</v>
+      </c>
+      <c r="M6" s="2">
+        <v>93</v>
+      </c>
+      <c r="N6" s="16">
+        <v>1</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="19">
+        <v>13</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G7" s="17">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>63</v>
+      </c>
+      <c r="M7" s="2">
+        <v>80</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="B8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19">
+        <v>147</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.435</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.245</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.122</v>
+      </c>
+      <c r="H8" s="17">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0.02</v>
+      </c>
+      <c r="J8" s="17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K8" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L8" s="2">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="M8" s="2">
+        <v>97</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
+      <c r="P8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="B9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="19">
+        <v>58</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.155</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0.155</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>56.6</v>
+      </c>
+      <c r="M9" s="2">
+        <v>81</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="B10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="19">
+        <v>58</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="H10" s="17">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I10" s="17">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J10" s="17">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K10" s="17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L10" s="2">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="M10" s="2">
+        <v>96</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="B11" t="s">
+        <v>374</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="19">
+        <v>62</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.129</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="M11" s="2">
+        <v>86</v>
+      </c>
+      <c r="N11" s="16">
+        <v>1</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>2</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="B12" t="s">
+        <v>376</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="19">
+        <v>87</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.161</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>60.9</v>
+      </c>
+      <c r="M12" s="2">
+        <v>83</v>
+      </c>
+      <c r="N12" s="16">
+        <v>1</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>3</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="B13" t="s">
+        <v>378</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="19">
+        <v>45</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G13" s="17">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0.111</v>
+      </c>
+      <c r="I13" s="17">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="J13" s="17">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="K13" s="17">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>67.2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>99</v>
+      </c>
+      <c r="N13" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0</v>
+      </c>
+      <c r="P13" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>416</v>
+      </c>
+      <c r="B14" t="s">
+        <v>379</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="19">
+        <v>89</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.247</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.36</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H14" s="17">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="I14" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J14" s="17">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>61.3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>82</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0</v>
+      </c>
+      <c r="P14" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="B15" t="s">
+        <v>381</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="19">
+        <v>97</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.371</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0.186</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0.155</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>62.9</v>
+      </c>
+      <c r="M15" s="2">
+        <v>86</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="B16" t="s">
+        <v>383</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="19">
+        <v>77</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.182</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G16" s="17">
+        <v>0.156</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>55.6</v>
+      </c>
+      <c r="M16" s="2">
+        <v>82</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="B17" t="s">
+        <v>393</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="19">
+        <v>73</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.26</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="G17" s="17">
+        <v>0.192</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0.11</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0.11</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="M17" s="2">
+        <v>95</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="B18" t="s">
+        <v>386</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="19">
+        <v>127</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="H18" s="17">
+        <v>0.157</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>6.3E-2</v>
+      </c>
+      <c r="K18" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L18" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="M18" s="2">
+        <v>92</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>388</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="19">
+        <v>66</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0.47</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0.121</v>
+      </c>
+      <c r="H19" s="17">
+        <v>0.182</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J19" s="17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>64.8</v>
+      </c>
+      <c r="M19" s="2">
+        <v>95</v>
+      </c>
+      <c r="N19" s="16">
+        <v>1</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0</v>
+      </c>
+      <c r="P19" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>2</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="B20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="19">
+        <v>48</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="H20" s="17">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>59.1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>87</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>1</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="B21" t="s">
+        <v>392</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="19">
+        <v>46</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.217</v>
+      </c>
+      <c r="G21" s="17">
+        <v>0.152</v>
+      </c>
+      <c r="H21" s="17">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0.152</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>61.3</v>
+      </c>
+      <c r="M21" s="2">
+        <v>96</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0</v>
+      </c>
+      <c r="P21" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>394</v>
+      </c>
+      <c r="B22" t="s">
+        <v>395</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="19">
+        <v>15</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G22" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H22" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>67.5</v>
+      </c>
+      <c r="M22" s="2">
+        <v>81</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0</v>
+      </c>
+      <c r="O22" s="16">
+        <v>0</v>
+      </c>
+      <c r="P22" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="B23" t="s">
+        <v>397</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="19">
+        <v>63</v>
+      </c>
+      <c r="E23" s="17">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="G23" s="17">
+        <v>0.254</v>
+      </c>
+      <c r="H23" s="17">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K23" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L23" s="2">
+        <v>63</v>
+      </c>
+      <c r="M23" s="2">
+        <v>89</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="O23" s="16">
+        <v>0</v>
+      </c>
+      <c r="P23" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="B24" t="s">
+        <v>399</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="19">
+        <v>62</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F24" s="17">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="G24" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H24" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I24" s="17">
+        <v>0</v>
+      </c>
+      <c r="J24" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K24" s="17">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="M24" s="2">
+        <v>83</v>
+      </c>
+      <c r="N24" s="16">
+        <v>1</v>
+      </c>
+      <c r="O24" s="16">
+        <v>0</v>
+      </c>
+      <c r="P24" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>2</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="B25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="19">
+        <v>85</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="F25" s="17">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="G25" s="17">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H25" s="17">
+        <v>0</v>
+      </c>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+      <c r="J25" s="17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K25" s="17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="L25" s="2">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="M25" s="2">
+        <v>84</v>
+      </c>
+      <c r="N25" s="16">
+        <v>1</v>
+      </c>
+      <c r="O25" s="16">
+        <v>0</v>
+      </c>
+      <c r="P25" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>3</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B26" t="s">
+        <v>403</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="19">
+        <v>38</v>
+      </c>
+      <c r="E26" s="17">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G26" s="17">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="K26" s="17">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="M26" s="2">
+        <v>82</v>
+      </c>
+      <c r="N26" s="16">
+        <v>1</v>
+      </c>
+      <c r="O26" s="16">
+        <v>0</v>
+      </c>
+      <c r="P26" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>2</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="B27" t="s">
+        <v>405</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="19">
+        <v>18</v>
+      </c>
+      <c r="E27" s="17">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F27" s="17">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G27" s="17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="K27" s="17">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="M27" s="2">
+        <v>77</v>
+      </c>
+      <c r="N27" s="16">
+        <v>1</v>
+      </c>
+      <c r="O27" s="16">
+        <v>0</v>
+      </c>
+      <c r="P27" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>2</v>
+      </c>
+      <c r="R27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="B28" t="s">
+        <v>407</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>35</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="F28" s="18">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G28" s="18">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H28" s="18">
+        <v>0</v>
+      </c>
+      <c r="I28" s="18">
+        <v>0</v>
+      </c>
+      <c r="J28" s="18">
+        <v>0</v>
+      </c>
+      <c r="K28" s="18">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="M28" s="1">
+        <v>79</v>
+      </c>
+      <c r="N28" s="16">
+        <v>1</v>
+      </c>
+      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+      <c r="P28" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>3</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="B29" t="s">
+        <v>409</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>22</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="F29" s="18">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0.318</v>
+      </c>
+      <c r="H29" s="18">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="I29" s="18">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K29" s="18">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>62</v>
+      </c>
+      <c r="M29" s="1">
+        <v>86</v>
+      </c>
+      <c r="N29" s="16">
+        <v>1</v>
+      </c>
+      <c r="O29" s="16">
+        <v>0</v>
+      </c>
+      <c r="P29" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>2</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="B30" t="s">
+        <v>411</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>60</v>
+      </c>
+      <c r="E30" s="18">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="F30" s="18">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G30" s="18">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="H30" s="18">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="I30" s="18">
+        <v>0</v>
+      </c>
+      <c r="J30" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="K30" s="18">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>62.1</v>
+      </c>
+      <c r="M30" s="1">
+        <v>93</v>
+      </c>
+      <c r="N30" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="O30" s="16">
+        <v>0</v>
+      </c>
+      <c r="P30" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>1</v>
+      </c>
+      <c r="R30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>412</v>
+      </c>
+      <c r="B31" t="s">
+        <v>413</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>49</v>
+      </c>
+      <c r="E31" s="18">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="F31" s="18">
+        <v>0.224</v>
+      </c>
+      <c r="G31" s="18">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="H31" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="I31" s="18">
+        <v>0</v>
+      </c>
+      <c r="J31" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="K31" s="18">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>68.8</v>
+      </c>
+      <c r="M31" s="1">
+        <v>90</v>
+      </c>
+      <c r="N31" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="O31" s="16">
+        <v>0</v>
+      </c>
+      <c r="P31" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>2</v>
+      </c>
+      <c r="R31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="B32" t="s">
+        <v>415</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>60</v>
+      </c>
+      <c r="E32" s="18">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="F32" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="G32" s="18">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="H32" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="I32" s="18">
+        <v>0</v>
+      </c>
+      <c r="J32" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="K32" s="18">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="M32" s="1">
+        <v>88</v>
+      </c>
+      <c r="N32" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O32" s="16">
+        <v>0</v>
+      </c>
+      <c r="P32" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>1</v>
+      </c>
+      <c r="R32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:R31" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1DA8C1-C587-45DF-87D3-9DC3B52B43A1}">
+  <dimension ref="A1:R32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1621,25 +3660,25 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -3177,7 +5216,6 @@
       </c>
     </row>
     <row r="29" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
       <c r="B29" s="22"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
@@ -3191,7 +5229,6 @@
       <c r="P29" s="16"/>
     </row>
     <row r="30" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
       <c r="B30" s="22"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
@@ -3205,7 +5242,6 @@
       <c r="P30" s="16"/>
     </row>
     <row r="31" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
       <c r="B31" s="22"/>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
@@ -3222,28 +5258,29 @@
       <c r="A32"/>
       <c r="C32"/>
       <c r="D32"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
       <c r="L32"/>
       <c r="M32"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
       <c r="Q32"/>
       <c r="R32"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R32" xr:uid="{9C1DA8C1-C587-45DF-87D3-9DC3B52B43A1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4289AE-5C21-47E6-BE9F-F3EB4C22DEB6}">
   <dimension ref="A1:R29"/>
   <sheetViews>
@@ -4900,6 +6937,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R29" xr:uid="{CA4289AE-5C21-47E6-BE9F-F3EB4C22DEB6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R29">
     <sortCondition ref="A2:A29"/>
   </sortState>
@@ -4908,7 +6946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B1F18-5F75-47B1-B429-DF58E6F9E79C}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -4916,7 +6954,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5904,11 +7942,12 @@
       <c r="P39" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R39" xr:uid="{E87B1F18-5F75-47B1-B429-DF58E6F9E79C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E33BB37-4D69-4A58-80FE-648AC47B185D}">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -5916,7 +7955,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q27" sqref="Q27"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7249,11 +9288,12 @@
       <c r="P37" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R37" xr:uid="{9E33BB37-4D69-4A58-80FE-648AC47B185D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -7261,7 +9301,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="A1:R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9267,6 +11307,7 @@
       <c r="P39" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R35" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R35">
     <sortCondition ref="A2:A35"/>
   </sortState>
@@ -9274,15 +11315,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD98AB24-8EFF-4477-9EFD-02014029C60E}">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="A1:R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11714,6 +13755,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R43" xr:uid="{CD98AB24-8EFF-4477-9EFD-02014029C60E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:XFD43">
     <sortCondition ref="A2:A43"/>
   </sortState>

</xml_diff>

<commit_message>
add PH department to database
</commit_message>
<xml_diff>
--- a/data/courses_data.xlsx
+++ b/data/courses_data.xlsx
@@ -8,27 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\course-finder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD7728E-06E4-4E0A-A4CF-E8C1EAD49AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302B8C12-4B17-4E40-B8A9-88C4F721CED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="2925" windowWidth="17610" windowHeight="15525" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
+    <workbookView xWindow="1590" yWindow="5850" windowWidth="17610" windowHeight="12600" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="ST - Statistics" sheetId="9" r:id="rId1"/>
-    <sheet name="IR - International Relations" sheetId="7" r:id="rId2"/>
-    <sheet name="MA - Mathematics" sheetId="6" r:id="rId3"/>
-    <sheet name="FM - Finance" sheetId="3" r:id="rId4"/>
-    <sheet name="MG - Management" sheetId="4" r:id="rId5"/>
-    <sheet name="EC - Economics" sheetId="2" r:id="rId6"/>
-    <sheet name="GV - Government" sheetId="1" r:id="rId7"/>
+    <sheet name="PH - Philosophy" sheetId="10" r:id="rId1"/>
+    <sheet name="ST - Statistics" sheetId="9" r:id="rId2"/>
+    <sheet name="IR - International Relations" sheetId="7" r:id="rId3"/>
+    <sheet name="MA - Mathematics" sheetId="6" r:id="rId4"/>
+    <sheet name="FM - Finance" sheetId="3" r:id="rId5"/>
+    <sheet name="MG - Management" sheetId="4" r:id="rId6"/>
+    <sheet name="EC - Economics" sheetId="2" r:id="rId7"/>
+    <sheet name="GV - Government" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'EC - Economics'!$A$1:$R$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FM - Finance'!$A$1:$R$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'GV - Government'!$A$1:$R$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'IR - International Relations'!$A$1:$R$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MA - Mathematics'!$A$1:$R$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'MG - Management'!$A$1:$R$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ST - Statistics'!$A$1:$R$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'EC - Economics'!$A$1:$R$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'FM - Finance'!$A$1:$R$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'GV - Government'!$A$1:$R$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'IR - International Relations'!$A$1:$R$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'MA - Mathematics'!$A$1:$R$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'MG - Management'!$A$1:$R$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PH - Philosophy'!$A$1:$R$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ST - Statistics'!$A$1:$R$31</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="459">
   <si>
     <t>Code</t>
   </si>
@@ -1302,6 +1304,132 @@
   </si>
   <si>
     <t>ST226</t>
+  </si>
+  <si>
+    <t>PH103</t>
+  </si>
+  <si>
+    <t>The Big Questions: An Introduction to Philosophy</t>
+  </si>
+  <si>
+    <t>PH105</t>
+  </si>
+  <si>
+    <t>Historical and Global Perspectives on Philosophy</t>
+  </si>
+  <si>
+    <t>PH111</t>
+  </si>
+  <si>
+    <t>Introduction to Logic</t>
+  </si>
+  <si>
+    <t>PH112</t>
+  </si>
+  <si>
+    <t>Intermediate Logic and Probability</t>
+  </si>
+  <si>
+    <t>PH201</t>
+  </si>
+  <si>
+    <t>Philosophy of Science</t>
+  </si>
+  <si>
+    <t>PH214</t>
+  </si>
+  <si>
+    <t>Philosophy, Morals and Politics</t>
+  </si>
+  <si>
+    <t>PH222</t>
+  </si>
+  <si>
+    <t>Philosophy and Public Policy</t>
+  </si>
+  <si>
+    <t>PH223</t>
+  </si>
+  <si>
+    <t>Mind and Metaphysics</t>
+  </si>
+  <si>
+    <t>PH224</t>
+  </si>
+  <si>
+    <t>Epistemology</t>
+  </si>
+  <si>
+    <t>PH225</t>
+  </si>
+  <si>
+    <t>Business and Organisational Ethics</t>
+  </si>
+  <si>
+    <t>PH226</t>
+  </si>
+  <si>
+    <t>Philosophy of Society</t>
+  </si>
+  <si>
+    <t>PH230</t>
+  </si>
+  <si>
+    <t>Einstein for Everyone: From Time Travel to the Edge of the Universe</t>
+  </si>
+  <si>
+    <t>PH232</t>
+  </si>
+  <si>
+    <t>Physics and Uncertainty: From Quantum Jumps to Stock Market Crashes</t>
+  </si>
+  <si>
+    <t>PH237</t>
+  </si>
+  <si>
+    <t>Advanced Logic</t>
+  </si>
+  <si>
+    <t>PH238</t>
+  </si>
+  <si>
+    <t>Philosophy of Language</t>
+  </si>
+  <si>
+    <t>PH239</t>
+  </si>
+  <si>
+    <t>Anarchy, Authority and Evidence: Topics in Philosophy of Law</t>
+  </si>
+  <si>
+    <t>PH240</t>
+  </si>
+  <si>
+    <t>The Ethics of Data and AI</t>
+  </si>
+  <si>
+    <t>PH311</t>
+  </si>
+  <si>
+    <t>Philosophy of Economics</t>
+  </si>
+  <si>
+    <t>PH333</t>
+  </si>
+  <si>
+    <t>Philosophy of Gender and Race</t>
+  </si>
+  <si>
+    <t>PH341</t>
+  </si>
+  <si>
+    <t>Philosophy, Politics and Economics: Applications</t>
+  </si>
+  <si>
+    <t>PH399</t>
+  </si>
+  <si>
+    <t>Dissertation in Philosophy</t>
   </si>
 </sst>
 </file>
@@ -1782,14 +1910,1401 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B627F1F-643B-4D6F-8A59-A585FB840C1F}">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>175</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0.36</v>
+      </c>
+      <c r="G2" s="18">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H2" s="18">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I2" s="18">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J2" s="18">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="K2" s="18">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>66.3</v>
+      </c>
+      <c r="M2" s="1">
+        <v>82</v>
+      </c>
+      <c r="N2" s="16">
+        <v>1</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>3</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>419</v>
+      </c>
+      <c r="B3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="19">
+        <v>76</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="G3" s="17">
+        <v>3.9E-2</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>0</v>
+      </c>
+      <c r="J3" s="17">
+        <v>3.9E-2</v>
+      </c>
+      <c r="K3" s="17">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>65.3</v>
+      </c>
+      <c r="M3" s="2">
+        <v>77</v>
+      </c>
+      <c r="N3" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="19">
+        <v>209</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="I4" s="17">
+        <v>2.4E-2</v>
+      </c>
+      <c r="J4" s="17">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="K4" s="17">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>58.9</v>
+      </c>
+      <c r="M4" s="2">
+        <v>94</v>
+      </c>
+      <c r="N4" s="16">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" t="s">
+        <v>424</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="19">
+        <v>40</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="H5" s="17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I5" s="17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J5" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="M5" s="2">
+        <v>89</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0</v>
+      </c>
+      <c r="P5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>425</v>
+      </c>
+      <c r="B6" t="s">
+        <v>426</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19">
+        <v>36</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G6" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>0</v>
+      </c>
+      <c r="K6" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>65.2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>72</v>
+      </c>
+      <c r="N6" s="16">
+        <v>1</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="B7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19">
+        <v>98</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="G7" s="17">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="L7" s="2">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="M7" s="2">
+        <v>77</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>429</v>
+      </c>
+      <c r="B8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19">
+        <v>87</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.379</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K8" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="M8" s="2">
+        <v>77</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P8" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>431</v>
+      </c>
+      <c r="B9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19">
+        <v>27</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.63</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0.111</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>65.3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>73</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>3</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="B10" t="s">
+        <v>434</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="19">
+        <v>46</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="G10" s="17">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>66.8</v>
+      </c>
+      <c r="M10" s="2">
+        <v>79</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="B11" t="s">
+        <v>436</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="19">
+        <v>115</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.496</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.113</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>68.8</v>
+      </c>
+      <c r="M11" s="2">
+        <v>80</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="B12" t="s">
+        <v>438</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="19">
+        <v>45</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="G12" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J12" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="M12" s="2">
+        <v>77</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="B13" t="s">
+        <v>440</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="19">
+        <v>35</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H13" s="17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K13" s="17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>60.1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>77</v>
+      </c>
+      <c r="N13" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P13" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="B14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="19">
+        <v>32</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.156</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="G14" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>3.1E-2</v>
+      </c>
+      <c r="J14" s="17">
+        <v>3.1E-2</v>
+      </c>
+      <c r="K14" s="17">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>62.7</v>
+      </c>
+      <c r="M14" s="2">
+        <v>74</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P14" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="B15" t="s">
+        <v>444</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="19">
+        <v>16</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="G15" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0.188</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="K15" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>62</v>
+      </c>
+      <c r="M15" s="2">
+        <v>78</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0</v>
+      </c>
+      <c r="P15" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="B16" t="s">
+        <v>446</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="19">
+        <v>41</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.317</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="G16" s="17">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="H16" s="17">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>63.4</v>
+      </c>
+      <c r="M16" s="2">
+        <v>75</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P16" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>2</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="B17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="19">
+        <v>45</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="G17" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>69.5</v>
+      </c>
+      <c r="M17" s="2">
+        <v>78</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" t="s">
+        <v>450</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="19">
+        <v>58</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="G18" s="17">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="H18" s="17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>66</v>
+      </c>
+      <c r="M18" s="2">
+        <v>74</v>
+      </c>
+      <c r="N18" s="16">
+        <v>1</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>2</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="B19" t="s">
+        <v>452</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="19">
+        <v>115</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.13</v>
+      </c>
+      <c r="G19" s="17">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H19" s="17">
+        <v>0</v>
+      </c>
+      <c r="I19" s="17">
+        <v>0</v>
+      </c>
+      <c r="J19" s="17">
+        <v>0</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="M19" s="2">
+        <v>83</v>
+      </c>
+      <c r="N19" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P19" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>3</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="B20" t="s">
+        <v>454</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="19">
+        <v>33</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="H20" s="17">
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>66.5</v>
+      </c>
+      <c r="M20" s="2">
+        <v>80</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2</v>
+      </c>
+      <c r="R20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" t="s">
+        <v>456</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19">
+        <v>51</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G21" s="17">
+        <v>0</v>
+      </c>
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="M21" s="2">
+        <v>80</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.85</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="P21" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>3</v>
+      </c>
+      <c r="R21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>457</v>
+      </c>
+      <c r="B22" t="s">
+        <v>458</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="19">
+        <v>33</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>65.3</v>
+      </c>
+      <c r="M22" s="2">
+        <v>77</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="O22" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="P22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>2</v>
+      </c>
+      <c r="R22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:R27" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S32" sqref="S32"/>
+      <selection pane="bottomRight" activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,7 +5121,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R31" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}"/>
@@ -3614,7 +5129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1DA8C1-C587-45DF-87D3-9DC3B52B43A1}">
   <dimension ref="A1:R32"/>
   <sheetViews>
@@ -5280,7 +6795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4289AE-5C21-47E6-BE9F-F3EB4C22DEB6}">
   <dimension ref="A1:R29"/>
   <sheetViews>
@@ -6946,7 +8461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B1F18-5F75-47B1-B429-DF58E6F9E79C}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -7947,7 +9462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E33BB37-4D69-4A58-80FE-648AC47B185D}">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -9293,7 +10808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -11315,7 +12830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD98AB24-8EFF-4477-9EFD-02014029C60E}">
   <dimension ref="A1:R43"/>
   <sheetViews>

</xml_diff>

<commit_message>
add LL department to database
</commit_message>
<xml_diff>
--- a/data/courses_data.xlsx
+++ b/data/courses_data.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\course-finder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302B8C12-4B17-4E40-B8A9-88C4F721CED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98160431-138B-421F-8864-4218B747B89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1590" yWindow="5850" windowWidth="17610" windowHeight="12600" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="PH - Philosophy" sheetId="10" r:id="rId1"/>
-    <sheet name="ST - Statistics" sheetId="9" r:id="rId2"/>
-    <sheet name="IR - International Relations" sheetId="7" r:id="rId3"/>
-    <sheet name="MA - Mathematics" sheetId="6" r:id="rId4"/>
-    <sheet name="FM - Finance" sheetId="3" r:id="rId5"/>
-    <sheet name="MG - Management" sheetId="4" r:id="rId6"/>
-    <sheet name="EC - Economics" sheetId="2" r:id="rId7"/>
-    <sheet name="GV - Government" sheetId="1" r:id="rId8"/>
+    <sheet name="LL - Law" sheetId="11" r:id="rId1"/>
+    <sheet name="PH - Philosophy" sheetId="10" r:id="rId2"/>
+    <sheet name="ST - Statistics" sheetId="9" r:id="rId3"/>
+    <sheet name="IR - International Relations" sheetId="7" r:id="rId4"/>
+    <sheet name="MA - Mathematics" sheetId="6" r:id="rId5"/>
+    <sheet name="FM - Finance" sheetId="3" r:id="rId6"/>
+    <sheet name="MG - Management" sheetId="4" r:id="rId7"/>
+    <sheet name="EC - Economics" sheetId="2" r:id="rId8"/>
+    <sheet name="GV - Government" sheetId="1" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'EC - Economics'!$A$1:$R$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'FM - Finance'!$A$1:$R$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'GV - Government'!$A$1:$R$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'IR - International Relations'!$A$1:$R$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'MA - Mathematics'!$A$1:$R$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'MG - Management'!$A$1:$R$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PH - Philosophy'!$A$1:$R$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ST - Statistics'!$A$1:$R$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'EC - Economics'!$A$1:$R$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'FM - Finance'!$A$1:$R$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'GV - Government'!$A$1:$R$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'IR - International Relations'!$A$1:$R$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LL - Law'!$A$1:$R$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'MA - Mathematics'!$A$1:$R$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MG - Management'!$A$1:$R$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PH - Philosophy'!$A$1:$R$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ST - Statistics'!$A$1:$R$31</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="531">
   <si>
     <t>Code</t>
   </si>
@@ -1430,6 +1432,222 @@
   </si>
   <si>
     <t>Dissertation in Philosophy</t>
+  </si>
+  <si>
+    <t>LL104</t>
+  </si>
+  <si>
+    <t>Law of Obligations</t>
+  </si>
+  <si>
+    <t>LL106</t>
+  </si>
+  <si>
+    <t>Public Law</t>
+  </si>
+  <si>
+    <t>LL108</t>
+  </si>
+  <si>
+    <t>Criminal Law</t>
+  </si>
+  <si>
+    <t>LL142</t>
+  </si>
+  <si>
+    <t>Contract Law</t>
+  </si>
+  <si>
+    <t>LL143</t>
+  </si>
+  <si>
+    <t>Tort Law</t>
+  </si>
+  <si>
+    <t>LL201</t>
+  </si>
+  <si>
+    <t>Law and State Power</t>
+  </si>
+  <si>
+    <t>LL202</t>
+  </si>
+  <si>
+    <t>Commercial Contracts</t>
+  </si>
+  <si>
+    <t>LL203</t>
+  </si>
+  <si>
+    <t>Company Law</t>
+  </si>
+  <si>
+    <t>LL204</t>
+  </si>
+  <si>
+    <t>Advanced Torts</t>
+  </si>
+  <si>
+    <t>LL205</t>
+  </si>
+  <si>
+    <t>Medical Law</t>
+  </si>
+  <si>
+    <t>LL207</t>
+  </si>
+  <si>
+    <t>Civil Liberties and Human Rights</t>
+  </si>
+  <si>
+    <t>LL208</t>
+  </si>
+  <si>
+    <t>Race, Class and Law</t>
+  </si>
+  <si>
+    <t>LL210</t>
+  </si>
+  <si>
+    <t>Information Technology and the Law</t>
+  </si>
+  <si>
+    <t>LL211</t>
+  </si>
+  <si>
+    <t>Law, Poverty and Access to Justice</t>
+  </si>
+  <si>
+    <t>LL212</t>
+  </si>
+  <si>
+    <t>Conflict of Laws</t>
+  </si>
+  <si>
+    <t>LL221</t>
+  </si>
+  <si>
+    <t>Family Law</t>
+  </si>
+  <si>
+    <t>LL232</t>
+  </si>
+  <si>
+    <t>Law and Institutions of the European Union</t>
+  </si>
+  <si>
+    <t>LL233</t>
+  </si>
+  <si>
+    <t>Law of Evidence</t>
+  </si>
+  <si>
+    <t>LL241</t>
+  </si>
+  <si>
+    <t>European Legal History</t>
+  </si>
+  <si>
+    <t>LL250</t>
+  </si>
+  <si>
+    <t>Law and the Environment</t>
+  </si>
+  <si>
+    <t>LL251</t>
+  </si>
+  <si>
+    <t>Intellectual Property Law</t>
+  </si>
+  <si>
+    <t>LL253</t>
+  </si>
+  <si>
+    <t>The Law of Corporate Insolvency</t>
+  </si>
+  <si>
+    <t>LL257</t>
+  </si>
+  <si>
+    <t>Employment Law</t>
+  </si>
+  <si>
+    <t>LL272</t>
+  </si>
+  <si>
+    <t>Outlines of Modern Criminology</t>
+  </si>
+  <si>
+    <t>LL275</t>
+  </si>
+  <si>
+    <t>Property II</t>
+  </si>
+  <si>
+    <t>LL278</t>
+  </si>
+  <si>
+    <t>Public International Law</t>
+  </si>
+  <si>
+    <t>LL284</t>
+  </si>
+  <si>
+    <t>Topics in Sentencing and Criminal Justice</t>
+  </si>
+  <si>
+    <t>LL293</t>
+  </si>
+  <si>
+    <t>Tax and Tax Avoidance</t>
+  </si>
+  <si>
+    <t>LL295</t>
+  </si>
+  <si>
+    <t>Media Law</t>
+  </si>
+  <si>
+    <t>LL300</t>
+  </si>
+  <si>
+    <t>Competition Law</t>
+  </si>
+  <si>
+    <t>LL302</t>
+  </si>
+  <si>
+    <t>Restitution for Unjust Enrichment</t>
+  </si>
+  <si>
+    <t>LL303</t>
+  </si>
+  <si>
+    <t>Cultural Heritage and Art Law</t>
+  </si>
+  <si>
+    <t>LL305</t>
+  </si>
+  <si>
+    <t>Jurisprudence</t>
+  </si>
+  <si>
+    <t>LL342</t>
+  </si>
+  <si>
+    <t>International Protection of Human Rights</t>
+  </si>
+  <si>
+    <t>LL398</t>
+  </si>
+  <si>
+    <t>Half-Unit Dissertation on an Approved Legal Topic</t>
+  </si>
+  <si>
+    <t>Full-Unit Dissertation on an Approved Legal Topic</t>
+  </si>
+  <si>
+    <t>LL399</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1574,7 +1792,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1910,10 +2131,2127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E073D194-2DD0-4C2F-847B-BBB0A0E709C3}">
+  <dimension ref="A1:R38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="S34" sqref="S34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19">
+        <v>22</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="G2" s="17">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="J2" s="17">
+        <v>0</v>
+      </c>
+      <c r="K2" s="17">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>60.2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>70</v>
+      </c>
+      <c r="N2" s="16">
+        <v>0</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19">
+        <v>152</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+      <c r="F3" s="17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K3" s="17">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>62.4</v>
+      </c>
+      <c r="M3" s="2">
+        <v>75</v>
+      </c>
+      <c r="N3" s="16">
+        <v>0</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0</v>
+      </c>
+      <c r="P3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" t="s">
+        <v>464</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="19">
+        <v>192</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="G4" s="17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="J4" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K4" s="17">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>61.4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>71</v>
+      </c>
+      <c r="N4" s="16">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19">
+        <v>162</v>
+      </c>
+      <c r="E5" s="17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F5" s="17">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G5" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0.877</v>
+      </c>
+      <c r="J5" s="17">
+        <v>0</v>
+      </c>
+      <c r="K5" s="17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>63.2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>72</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0</v>
+      </c>
+      <c r="P5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19">
+        <v>146</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="J6" s="17">
+        <v>2.7E-2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>62.9</v>
+      </c>
+      <c r="M6" s="2">
+        <v>74</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19">
+        <v>13</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.308</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0.154</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>65.8</v>
+      </c>
+      <c r="M7" s="2">
+        <v>73</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="B8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19">
+        <v>88</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="H8" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
+        <v>0</v>
+      </c>
+      <c r="K8" s="17">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>64</v>
+      </c>
+      <c r="M8" s="2">
+        <v>73</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
+      <c r="P8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="B9" t="s">
+        <v>474</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19">
+        <v>88</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.307</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="G9" s="17">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>66.5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>73</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0</v>
+      </c>
+      <c r="P9" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="B10" t="s">
+        <v>476</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G10" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>66.3</v>
+      </c>
+      <c r="M10" s="2">
+        <v>72</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="B11" t="s">
+        <v>478</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="19">
+        <v>88</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.17</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.114</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="29">
+        <v>64.7</v>
+      </c>
+      <c r="M11" s="29">
+        <v>73</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="B12" t="s">
+        <v>480</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19">
+        <v>21</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H12" s="17">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0</v>
+      </c>
+      <c r="L12" s="29">
+        <v>64.2</v>
+      </c>
+      <c r="M12" s="29">
+        <v>75</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0</v>
+      </c>
+      <c r="P12" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="B13" t="s">
+        <v>482</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="19">
+        <v>24</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="G13" s="17">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H13" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0</v>
+      </c>
+      <c r="K13" s="17">
+        <v>0</v>
+      </c>
+      <c r="L13" s="29">
+        <v>67.2</v>
+      </c>
+      <c r="M13" s="29">
+        <v>80</v>
+      </c>
+      <c r="N13" s="16">
+        <v>1</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0</v>
+      </c>
+      <c r="P13" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="B14" t="s">
+        <v>484</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19">
+        <v>55</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.182</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.745</v>
+      </c>
+      <c r="G14" s="17">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="29">
+        <v>65.5</v>
+      </c>
+      <c r="M14" s="29">
+        <v>73</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0</v>
+      </c>
+      <c r="P14" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="B15" t="s">
+        <v>486</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="19">
+        <v>20</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0</v>
+      </c>
+      <c r="L15" s="29">
+        <v>66.2</v>
+      </c>
+      <c r="M15" s="29">
+        <v>71</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0</v>
+      </c>
+      <c r="P15" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="B16" t="s">
+        <v>488</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19">
+        <v>23</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="G16" s="17">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0</v>
+      </c>
+      <c r="L16" s="29">
+        <v>66.2</v>
+      </c>
+      <c r="M16" s="29">
+        <v>73</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="B17" t="s">
+        <v>490</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>64</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="G17" s="17">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="H17" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="29">
+        <v>63.9</v>
+      </c>
+      <c r="M17" s="29">
+        <v>72</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="B18" t="s">
+        <v>492</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19">
+        <v>165</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0.182</v>
+      </c>
+      <c r="H18" s="17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0</v>
+      </c>
+      <c r="L18" s="29">
+        <v>63.3</v>
+      </c>
+      <c r="M18" s="29">
+        <v>75</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="B19" t="s">
+        <v>494</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="19">
+        <v>30</v>
+      </c>
+      <c r="E19" s="17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="17">
+        <v>0</v>
+      </c>
+      <c r="I19" s="17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="J19" s="17">
+        <v>0</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0</v>
+      </c>
+      <c r="L19" s="29">
+        <v>61.5</v>
+      </c>
+      <c r="M19" s="29">
+        <v>71</v>
+      </c>
+      <c r="N19" s="16">
+        <v>0</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0</v>
+      </c>
+      <c r="P19" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>495</v>
+      </c>
+      <c r="B20" t="s">
+        <v>496</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="19">
+        <v>4</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0</v>
+      </c>
+      <c r="H20" s="17">
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+      <c r="L20" s="29">
+        <v>67.5</v>
+      </c>
+      <c r="M20" s="29">
+        <v>71</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0</v>
+      </c>
+      <c r="P20" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>497</v>
+      </c>
+      <c r="B21" t="s">
+        <v>498</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19">
+        <v>22</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="17">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="29">
+        <v>62</v>
+      </c>
+      <c r="M21" s="29">
+        <v>74</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0</v>
+      </c>
+      <c r="P21" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="B22" t="s">
+        <v>500</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>36</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="F22" s="18">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="G22" s="18">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="H22" s="18">
+        <v>0</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0</v>
+      </c>
+      <c r="K22" s="18">
+        <v>0</v>
+      </c>
+      <c r="L22" s="30">
+        <v>67.2</v>
+      </c>
+      <c r="M22" s="30">
+        <v>74</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0</v>
+      </c>
+      <c r="O22" s="16">
+        <v>0</v>
+      </c>
+      <c r="P22" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>501</v>
+      </c>
+      <c r="B23" t="s">
+        <v>502</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>20</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H23" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0</v>
+      </c>
+      <c r="J23" s="18">
+        <v>0</v>
+      </c>
+      <c r="K23" s="18">
+        <v>0</v>
+      </c>
+      <c r="L23" s="30">
+        <v>64.5</v>
+      </c>
+      <c r="M23" s="30">
+        <v>74</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0</v>
+      </c>
+      <c r="O23" s="16">
+        <v>0</v>
+      </c>
+      <c r="P23" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="B24" t="s">
+        <v>504</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>25</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="F24" s="18">
+        <v>0.76</v>
+      </c>
+      <c r="G24" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="H24" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="I24" s="18">
+        <v>0</v>
+      </c>
+      <c r="J24" s="18">
+        <v>0</v>
+      </c>
+      <c r="K24" s="18">
+        <v>0</v>
+      </c>
+      <c r="L24" s="30">
+        <v>64.2</v>
+      </c>
+      <c r="M24" s="30">
+        <v>71</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0</v>
+      </c>
+      <c r="O24" s="16">
+        <v>0</v>
+      </c>
+      <c r="P24" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>505</v>
+      </c>
+      <c r="B25" t="s">
+        <v>506</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0.222</v>
+      </c>
+      <c r="F25" s="18">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="G25" s="18">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0</v>
+      </c>
+      <c r="I25" s="18">
+        <v>0</v>
+      </c>
+      <c r="J25" s="18">
+        <v>0</v>
+      </c>
+      <c r="K25" s="18">
+        <v>0</v>
+      </c>
+      <c r="L25" s="30">
+        <v>64.7</v>
+      </c>
+      <c r="M25" s="30">
+        <v>71</v>
+      </c>
+      <c r="N25" s="16">
+        <v>0</v>
+      </c>
+      <c r="O25" s="16">
+        <v>0</v>
+      </c>
+      <c r="P25" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0</v>
+      </c>
+      <c r="R25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="B26" t="s">
+        <v>508</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>198</v>
+      </c>
+      <c r="E26" s="18">
+        <v>0.126</v>
+      </c>
+      <c r="F26" s="18">
+        <v>0.621</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H26" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="I26" s="18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J26" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K26" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L26" s="30">
+        <v>62.1</v>
+      </c>
+      <c r="M26" s="30">
+        <v>75</v>
+      </c>
+      <c r="N26" s="16">
+        <v>0</v>
+      </c>
+      <c r="O26" s="16">
+        <v>0</v>
+      </c>
+      <c r="P26" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>509</v>
+      </c>
+      <c r="B27" t="s">
+        <v>510</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>56</v>
+      </c>
+      <c r="E27" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F27" s="18">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="G27" s="18">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H27" s="18">
+        <v>0</v>
+      </c>
+      <c r="I27" s="18">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
+        <v>0</v>
+      </c>
+      <c r="K27" s="18">
+        <v>0</v>
+      </c>
+      <c r="L27" s="30">
+        <v>66.3</v>
+      </c>
+      <c r="M27" s="30">
+        <v>74</v>
+      </c>
+      <c r="N27" s="16">
+        <v>0</v>
+      </c>
+      <c r="O27" s="16">
+        <v>0</v>
+      </c>
+      <c r="P27" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>0</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="B28" t="s">
+        <v>512</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>13</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0.154</v>
+      </c>
+      <c r="F28" s="18">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="G28" s="18">
+        <v>0.154</v>
+      </c>
+      <c r="H28" s="18">
+        <v>0</v>
+      </c>
+      <c r="I28" s="18">
+        <v>0</v>
+      </c>
+      <c r="J28" s="18">
+        <v>0</v>
+      </c>
+      <c r="K28" s="18">
+        <v>0</v>
+      </c>
+      <c r="L28" s="30">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="M28" s="30">
+        <v>73</v>
+      </c>
+      <c r="N28" s="16">
+        <v>0</v>
+      </c>
+      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+      <c r="P28" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>0</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="B29" t="s">
+        <v>514</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>26</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F29" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="18">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="H29" s="18">
+        <v>0</v>
+      </c>
+      <c r="I29" s="18">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K29" s="18">
+        <v>0</v>
+      </c>
+      <c r="L29" s="30">
+        <v>65</v>
+      </c>
+      <c r="M29" s="30">
+        <v>73</v>
+      </c>
+      <c r="N29" s="16">
+        <v>0</v>
+      </c>
+      <c r="O29" s="16">
+        <v>0</v>
+      </c>
+      <c r="P29" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>0</v>
+      </c>
+      <c r="R29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="B30" t="s">
+        <v>516</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>24</v>
+      </c>
+      <c r="E30" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F30" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="18">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H30" s="18">
+        <v>0</v>
+      </c>
+      <c r="I30" s="18">
+        <v>0</v>
+      </c>
+      <c r="J30" s="18">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="K30" s="18">
+        <v>0</v>
+      </c>
+      <c r="L30" s="30">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="M30" s="30">
+        <v>73</v>
+      </c>
+      <c r="N30" s="16">
+        <v>1</v>
+      </c>
+      <c r="O30" s="16">
+        <v>0</v>
+      </c>
+      <c r="P30" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>1</v>
+      </c>
+      <c r="R30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>517</v>
+      </c>
+      <c r="B31" t="s">
+        <v>518</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>36</v>
+      </c>
+      <c r="E31" s="18">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F31" s="18">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="G31" s="18">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="H31" s="18">
+        <v>0</v>
+      </c>
+      <c r="I31" s="18">
+        <v>0</v>
+      </c>
+      <c r="J31" s="18">
+        <v>0</v>
+      </c>
+      <c r="K31" s="18">
+        <v>0</v>
+      </c>
+      <c r="L31" s="30">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="M31" s="30">
+        <v>73</v>
+      </c>
+      <c r="N31" s="16">
+        <v>0</v>
+      </c>
+      <c r="O31" s="16">
+        <v>0</v>
+      </c>
+      <c r="P31" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>0</v>
+      </c>
+      <c r="R31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="B32" t="s">
+        <v>520</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4</v>
+      </c>
+      <c r="E32" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="G32" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="H32" s="18">
+        <v>0</v>
+      </c>
+      <c r="I32" s="18">
+        <v>0</v>
+      </c>
+      <c r="J32" s="18">
+        <v>0</v>
+      </c>
+      <c r="K32" s="18">
+        <v>0</v>
+      </c>
+      <c r="L32" s="30">
+        <v>66.5</v>
+      </c>
+      <c r="M32" s="30">
+        <v>71</v>
+      </c>
+      <c r="N32" s="16">
+        <v>0</v>
+      </c>
+      <c r="O32" s="16">
+        <v>0</v>
+      </c>
+      <c r="P32" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>0</v>
+      </c>
+      <c r="R32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="B33" t="s">
+        <v>522</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9</v>
+      </c>
+      <c r="E33" s="18">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F33" s="18">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="G33" s="18">
+        <v>0</v>
+      </c>
+      <c r="H33" s="18">
+        <v>0</v>
+      </c>
+      <c r="I33" s="18">
+        <v>0</v>
+      </c>
+      <c r="J33" s="18">
+        <v>0</v>
+      </c>
+      <c r="K33" s="18">
+        <v>0</v>
+      </c>
+      <c r="L33" s="30">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="M33" s="30">
+        <v>73</v>
+      </c>
+      <c r="N33" s="16">
+        <v>0</v>
+      </c>
+      <c r="O33" s="16">
+        <v>0</v>
+      </c>
+      <c r="P33" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>0</v>
+      </c>
+      <c r="R33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="B34" t="s">
+        <v>524</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>164</v>
+      </c>
+      <c r="E34" s="18">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="F34" s="18">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="G34" s="18">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="H34" s="18">
+        <v>0</v>
+      </c>
+      <c r="I34" s="18">
+        <v>0</v>
+      </c>
+      <c r="J34" s="18">
+        <v>0</v>
+      </c>
+      <c r="K34" s="18">
+        <v>0</v>
+      </c>
+      <c r="L34" s="30">
+        <v>65.5</v>
+      </c>
+      <c r="M34" s="30">
+        <v>76</v>
+      </c>
+      <c r="N34" s="16">
+        <v>0</v>
+      </c>
+      <c r="O34" s="16">
+        <v>0</v>
+      </c>
+      <c r="P34" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>0</v>
+      </c>
+      <c r="R34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="B35" t="s">
+        <v>526</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>11</v>
+      </c>
+      <c r="E35" s="18">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="F35" s="18">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G35" s="18">
+        <v>0</v>
+      </c>
+      <c r="H35" s="18">
+        <v>0</v>
+      </c>
+      <c r="I35" s="18">
+        <v>0</v>
+      </c>
+      <c r="J35" s="18">
+        <v>0</v>
+      </c>
+      <c r="K35" s="18">
+        <v>0</v>
+      </c>
+      <c r="L35" s="30">
+        <v>69.5</v>
+      </c>
+      <c r="M35" s="30">
+        <v>74</v>
+      </c>
+      <c r="N35" s="16">
+        <v>0</v>
+      </c>
+      <c r="O35" s="16">
+        <v>0</v>
+      </c>
+      <c r="P35" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>0</v>
+      </c>
+      <c r="R35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="B36" t="s">
+        <v>528</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+      <c r="E36" s="18">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F36" s="18">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G36" s="18">
+        <v>0</v>
+      </c>
+      <c r="H36" s="18">
+        <v>0</v>
+      </c>
+      <c r="I36" s="18">
+        <v>0</v>
+      </c>
+      <c r="J36" s="18">
+        <v>0</v>
+      </c>
+      <c r="K36" s="18">
+        <v>0</v>
+      </c>
+      <c r="L36" s="30">
+        <v>70</v>
+      </c>
+      <c r="M36" s="30">
+        <v>73</v>
+      </c>
+      <c r="N36" s="16">
+        <v>1</v>
+      </c>
+      <c r="O36" s="16">
+        <v>0</v>
+      </c>
+      <c r="P36" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>1</v>
+      </c>
+      <c r="R36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="B37" t="s">
+        <v>529</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>25</v>
+      </c>
+      <c r="E37" s="18">
+        <v>0.76</v>
+      </c>
+      <c r="F37" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="G37" s="18">
+        <v>0</v>
+      </c>
+      <c r="H37" s="18">
+        <v>0</v>
+      </c>
+      <c r="I37" s="18">
+        <v>0</v>
+      </c>
+      <c r="J37" s="18">
+        <v>0</v>
+      </c>
+      <c r="K37" s="18">
+        <v>0</v>
+      </c>
+      <c r="L37" s="30">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="M37" s="30">
+        <v>80</v>
+      </c>
+      <c r="N37" s="16">
+        <v>1</v>
+      </c>
+      <c r="O37" s="16">
+        <v>0</v>
+      </c>
+      <c r="P37" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>1</v>
+      </c>
+      <c r="R37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:R24" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B627F1F-643B-4D6F-8A59-A585FB840C1F}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -3174,7 +5512,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="19"/>
       <c r="E23" s="17"/>
@@ -3193,7 +5531,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="18"/>
@@ -3212,7 +5550,7 @@
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="18"/>
@@ -3231,7 +5569,7 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="18"/>
@@ -3250,7 +5588,7 @@
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="18"/>
@@ -3269,7 +5607,7 @@
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="18"/>
@@ -3296,7 +5634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBF643C-A3D3-4EB5-985C-EC2DDC2C341F}">
   <dimension ref="A1:R33"/>
   <sheetViews>
@@ -5129,7 +7467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1DA8C1-C587-45DF-87D3-9DC3B52B43A1}">
   <dimension ref="A1:R32"/>
   <sheetViews>
@@ -6795,7 +9133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4289AE-5C21-47E6-BE9F-F3EB4C22DEB6}">
   <dimension ref="A1:R29"/>
   <sheetViews>
@@ -8461,7 +10799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B1F18-5F75-47B1-B429-DF58E6F9E79C}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -9462,7 +11800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E33BB37-4D69-4A58-80FE-648AC47B185D}">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -10808,7 +13146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -12830,7 +15168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD98AB24-8EFF-4477-9EFD-02014029C60E}">
   <dimension ref="A1:R43"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix: EC department percentages
</commit_message>
<xml_diff>
--- a/data/courses_data.xlsx
+++ b/data/courses_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubois\Desktop\course-finder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98160431-138B-421F-8864-4218B747B89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA98E48-22B4-4156-A33C-83FCE300CBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="5850" windowWidth="17610" windowHeight="12600" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
+    <workbookView xWindow="1935" yWindow="6195" windowWidth="17610" windowHeight="12600" firstSheet="5" activeTab="7" xr2:uid="{DC73EE2F-9994-41D4-8CE7-61459B800A97}"/>
   </bookViews>
   <sheets>
     <sheet name="LL - Law" sheetId="11" r:id="rId1"/>
@@ -1714,7 +1714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1790,12 +1790,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2134,7 +2128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E073D194-2DD0-4C2F-847B-BBB0A0E709C3}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -2756,10 +2750,10 @@
       <c r="K11" s="17">
         <v>0</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="2">
         <v>64.7</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="2">
         <v>73</v>
       </c>
       <c r="N11" s="16">
@@ -2812,10 +2806,10 @@
       <c r="K12" s="17">
         <v>0</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="2">
         <v>64.2</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="2">
         <v>75</v>
       </c>
       <c r="N12" s="16">
@@ -2868,10 +2862,10 @@
       <c r="K13" s="17">
         <v>0</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="2">
         <v>67.2</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="2">
         <v>80</v>
       </c>
       <c r="N13" s="16">
@@ -2924,10 +2918,10 @@
       <c r="K14" s="17">
         <v>0</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="2">
         <v>65.5</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="2">
         <v>73</v>
       </c>
       <c r="N14" s="16">
@@ -2980,10 +2974,10 @@
       <c r="K15" s="17">
         <v>0</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="2">
         <v>66.2</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="2">
         <v>71</v>
       </c>
       <c r="N15" s="16">
@@ -3036,10 +3030,10 @@
       <c r="K16" s="17">
         <v>0</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="2">
         <v>66.2</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="2">
         <v>73</v>
       </c>
       <c r="N16" s="16">
@@ -3092,10 +3086,10 @@
       <c r="K17" s="17">
         <v>0</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="2">
         <v>63.9</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="2">
         <v>72</v>
       </c>
       <c r="N17" s="16">
@@ -3148,10 +3142,10 @@
       <c r="K18" s="17">
         <v>0</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="2">
         <v>63.3</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="2">
         <v>75</v>
       </c>
       <c r="N18" s="16">
@@ -3204,10 +3198,10 @@
       <c r="K19" s="17">
         <v>0</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="2">
         <v>61.5</v>
       </c>
-      <c r="M19" s="29">
+      <c r="M19" s="2">
         <v>71</v>
       </c>
       <c r="N19" s="16">
@@ -3260,10 +3254,10 @@
       <c r="K20" s="17">
         <v>0</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="2">
         <v>67.5</v>
       </c>
-      <c r="M20" s="29">
+      <c r="M20" s="2">
         <v>71</v>
       </c>
       <c r="N20" s="16">
@@ -3316,10 +3310,10 @@
       <c r="K21" s="17">
         <v>0</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="2">
         <v>62</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="2">
         <v>74</v>
       </c>
       <c r="N21" s="16">
@@ -3372,10 +3366,10 @@
       <c r="K22" s="18">
         <v>0</v>
       </c>
-      <c r="L22" s="30">
+      <c r="L22" s="1">
         <v>67.2</v>
       </c>
-      <c r="M22" s="30">
+      <c r="M22" s="1">
         <v>74</v>
       </c>
       <c r="N22" s="16">
@@ -3428,10 +3422,10 @@
       <c r="K23" s="18">
         <v>0</v>
       </c>
-      <c r="L23" s="30">
+      <c r="L23" s="1">
         <v>64.5</v>
       </c>
-      <c r="M23" s="30">
+      <c r="M23" s="1">
         <v>74</v>
       </c>
       <c r="N23" s="16">
@@ -3484,10 +3478,10 @@
       <c r="K24" s="18">
         <v>0</v>
       </c>
-      <c r="L24" s="30">
+      <c r="L24" s="1">
         <v>64.2</v>
       </c>
-      <c r="M24" s="30">
+      <c r="M24" s="1">
         <v>71</v>
       </c>
       <c r="N24" s="16">
@@ -3540,10 +3534,10 @@
       <c r="K25" s="18">
         <v>0</v>
       </c>
-      <c r="L25" s="30">
+      <c r="L25" s="1">
         <v>64.7</v>
       </c>
-      <c r="M25" s="30">
+      <c r="M25" s="1">
         <v>71</v>
       </c>
       <c r="N25" s="16">
@@ -3596,10 +3590,10 @@
       <c r="K26" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L26" s="30">
+      <c r="L26" s="1">
         <v>62.1</v>
       </c>
-      <c r="M26" s="30">
+      <c r="M26" s="1">
         <v>75</v>
       </c>
       <c r="N26" s="16">
@@ -3652,10 +3646,10 @@
       <c r="K27" s="18">
         <v>0</v>
       </c>
-      <c r="L27" s="30">
+      <c r="L27" s="1">
         <v>66.3</v>
       </c>
-      <c r="M27" s="30">
+      <c r="M27" s="1">
         <v>74</v>
       </c>
       <c r="N27" s="16">
@@ -3708,10 +3702,10 @@
       <c r="K28" s="18">
         <v>0</v>
       </c>
-      <c r="L28" s="30">
+      <c r="L28" s="1">
         <v>64.099999999999994</v>
       </c>
-      <c r="M28" s="30">
+      <c r="M28" s="1">
         <v>73</v>
       </c>
       <c r="N28" s="16">
@@ -3764,10 +3758,10 @@
       <c r="K29" s="18">
         <v>0</v>
       </c>
-      <c r="L29" s="30">
+      <c r="L29" s="1">
         <v>65</v>
       </c>
-      <c r="M29" s="30">
+      <c r="M29" s="1">
         <v>73</v>
       </c>
       <c r="N29" s="16">
@@ -3820,10 +3814,10 @@
       <c r="K30" s="18">
         <v>0</v>
       </c>
-      <c r="L30" s="30">
+      <c r="L30" s="1">
         <v>64.099999999999994</v>
       </c>
-      <c r="M30" s="30">
+      <c r="M30" s="1">
         <v>73</v>
       </c>
       <c r="N30" s="16">
@@ -3876,10 +3870,10 @@
       <c r="K31" s="18">
         <v>0</v>
       </c>
-      <c r="L31" s="30">
+      <c r="L31" s="1">
         <v>64.099999999999994</v>
       </c>
-      <c r="M31" s="30">
+      <c r="M31" s="1">
         <v>73</v>
       </c>
       <c r="N31" s="16">
@@ -3932,10 +3926,10 @@
       <c r="K32" s="18">
         <v>0</v>
       </c>
-      <c r="L32" s="30">
+      <c r="L32" s="1">
         <v>66.5</v>
       </c>
-      <c r="M32" s="30">
+      <c r="M32" s="1">
         <v>71</v>
       </c>
       <c r="N32" s="16">
@@ -3988,10 +3982,10 @@
       <c r="K33" s="18">
         <v>0</v>
       </c>
-      <c r="L33" s="30">
+      <c r="L33" s="1">
         <v>69.099999999999994</v>
       </c>
-      <c r="M33" s="30">
+      <c r="M33" s="1">
         <v>73</v>
       </c>
       <c r="N33" s="16">
@@ -4044,10 +4038,10 @@
       <c r="K34" s="18">
         <v>0</v>
       </c>
-      <c r="L34" s="30">
+      <c r="L34" s="1">
         <v>65.5</v>
       </c>
-      <c r="M34" s="30">
+      <c r="M34" s="1">
         <v>76</v>
       </c>
       <c r="N34" s="16">
@@ -4100,10 +4094,10 @@
       <c r="K35" s="18">
         <v>0</v>
       </c>
-      <c r="L35" s="30">
+      <c r="L35" s="1">
         <v>69.5</v>
       </c>
-      <c r="M35" s="30">
+      <c r="M35" s="1">
         <v>74</v>
       </c>
       <c r="N35" s="16">
@@ -4156,10 +4150,10 @@
       <c r="K36" s="18">
         <v>0</v>
       </c>
-      <c r="L36" s="30">
+      <c r="L36" s="1">
         <v>70</v>
       </c>
-      <c r="M36" s="30">
+      <c r="M36" s="1">
         <v>73</v>
       </c>
       <c r="N36" s="16">
@@ -4212,10 +4206,10 @@
       <c r="K37" s="18">
         <v>0</v>
       </c>
-      <c r="L37" s="30">
+      <c r="L37" s="1">
         <v>71.400000000000006</v>
       </c>
-      <c r="M37" s="30">
+      <c r="M37" s="1">
         <v>80</v>
       </c>
       <c r="N37" s="16">
@@ -13150,11 +13144,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16872B7-F2AA-41D3-8F3E-60BE21A6A82E}">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="A1:R35"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>